<commit_message>
update the response and figures
</commit_message>
<xml_diff>
--- a/figure/OperatorWeights.xlsx
+++ b/figure/OperatorWeights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanzhang/Documents/UOALearning/OperatorPaper/figure/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F34F1B8-5C4C-5449-8294-4E8C967A66E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60402D72-3B4F-3745-8307-9066AE7E8A64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="1040" windowWidth="33180" windowHeight="17440" activeTab="1" xr2:uid="{3FB4DF38-F6E0-1E40-BC74-3A8B570BED1B}"/>
+    <workbookView xWindow="35820" yWindow="1400" windowWidth="33180" windowHeight="17440" xr2:uid="{3FB4DF38-F6E0-1E40-BC74-3A8B570BED1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Absolute" sheetId="1" r:id="rId1"/>
@@ -147,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -170,6 +170,13 @@
     </font>
     <font>
       <sz val="24"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -346,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,47 +373,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -415,12 +395,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -469,6 +443,44 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A310927F-C9A1-4443-B16F-5623ACA02806}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -815,46 +827,46 @@
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="10" t="s">
+      <c r="D1" s="47"/>
+      <c r="E1" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="44"/>
+      <c r="G1" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="10" t="s">
+      <c r="H1" s="44"/>
+      <c r="I1" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="11"/>
+      <c r="J1" s="40"/>
     </row>
     <row r="2" spans="1:10" ht="31">
       <c r="C2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="15" t="s">
         <v>24</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="10" t="s">
         <v>24</v>
       </c>
       <c r="I2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -868,25 +880,25 @@
       <c r="C3" s="8">
         <v>25</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="15">
         <v>0</v>
       </c>
       <c r="E3" s="8">
         <v>25</v>
       </c>
-      <c r="F3" s="15">
-        <v>0</v>
-      </c>
-      <c r="G3" s="19">
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+      <c r="G3" s="12">
         <v>25</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="10">
         <v>0</v>
       </c>
       <c r="I3" s="8">
-        <v>25</v>
-      </c>
-      <c r="J3" s="12">
+        <v>20</v>
+      </c>
+      <c r="J3" s="9">
         <v>0</v>
       </c>
     </row>
@@ -898,25 +910,25 @@
       <c r="C4" s="8">
         <v>15</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="15">
         <v>30</v>
       </c>
       <c r="E4" s="8">
         <v>15</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="10">
         <v>30</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="12">
         <v>15</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="10">
         <v>30</v>
       </c>
-      <c r="I4" s="8">
-        <v>10</v>
-      </c>
-      <c r="J4" s="12">
+      <c r="I4" s="51">
+        <v>20</v>
+      </c>
+      <c r="J4" s="9">
         <v>30</v>
       </c>
     </row>
@@ -925,22 +937,22 @@
       <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="10">
-        <v>3</v>
-      </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="10">
-        <v>3</v>
-      </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="18">
-        <v>3</v>
-      </c>
-      <c r="H5" s="14"/>
+      <c r="C5" s="39">
+        <v>3</v>
+      </c>
+      <c r="D5" s="47"/>
+      <c r="E5" s="39">
+        <v>3</v>
+      </c>
+      <c r="F5" s="44"/>
+      <c r="G5" s="43">
+        <v>3</v>
+      </c>
+      <c r="H5" s="44"/>
       <c r="I5" s="8">
         <v>3</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="9">
         <v>3</v>
       </c>
     </row>
@@ -948,95 +960,97 @@
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="10">
-        <v>0</v>
-      </c>
-      <c r="D6" s="23"/>
+      <c r="C6" s="39">
+        <v>0</v>
+      </c>
+      <c r="D6" s="47"/>
       <c r="E6" s="8">
         <v>4</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="10">
         <v>1</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="12">
         <v>1</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="10">
         <v>1</v>
       </c>
-      <c r="I6" s="10">
-        <v>0</v>
-      </c>
-      <c r="J6" s="11"/>
+      <c r="I6" s="39">
+        <v>0</v>
+      </c>
+      <c r="J6" s="40"/>
     </row>
     <row r="7" spans="1:10" ht="31">
       <c r="B7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="10">
-        <v>0</v>
-      </c>
-      <c r="D7" s="23"/>
+      <c r="C7" s="39">
+        <v>0</v>
+      </c>
+      <c r="D7" s="47"/>
       <c r="E7" s="8">
         <v>5</v>
       </c>
-      <c r="F7" s="15">
-        <v>3</v>
-      </c>
-      <c r="G7" s="19">
-        <v>3</v>
-      </c>
-      <c r="H7" s="15">
-        <v>3</v>
-      </c>
-      <c r="I7" s="10">
-        <v>0</v>
-      </c>
-      <c r="J7" s="11"/>
+      <c r="F7" s="10">
+        <v>3</v>
+      </c>
+      <c r="G7" s="12">
+        <v>3</v>
+      </c>
+      <c r="H7" s="10">
+        <v>3</v>
+      </c>
+      <c r="I7" s="39">
+        <v>0</v>
+      </c>
+      <c r="J7" s="40"/>
     </row>
     <row r="8" spans="1:10" ht="31">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="10">
-        <v>3</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="10">
-        <v>3</v>
-      </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="18">
-        <v>3</v>
-      </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="10">
+      <c r="C8" s="39">
+        <v>3</v>
+      </c>
+      <c r="D8" s="47"/>
+      <c r="E8" s="39">
+        <v>3</v>
+      </c>
+      <c r="F8" s="44"/>
+      <c r="G8" s="43">
+        <v>3</v>
+      </c>
+      <c r="H8" s="44"/>
+      <c r="I8" s="52">
+        <v>5</v>
+      </c>
+      <c r="J8" s="50">
         <v>10</v>
       </c>
-      <c r="J8" s="11"/>
     </row>
     <row r="9" spans="1:10" ht="31">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="10">
-        <v>3</v>
-      </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="10">
-        <v>3</v>
-      </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="18">
-        <v>3</v>
-      </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="10">
+      <c r="C9" s="39">
+        <v>3</v>
+      </c>
+      <c r="D9" s="47"/>
+      <c r="E9" s="39">
+        <v>3</v>
+      </c>
+      <c r="F9" s="44"/>
+      <c r="G9" s="43">
+        <v>3</v>
+      </c>
+      <c r="H9" s="44"/>
+      <c r="I9" s="39">
         <v>5</v>
       </c>
-      <c r="J9" s="11"/>
+      <c r="J9" s="40"/>
     </row>
     <row r="10" spans="1:10" ht="31">
       <c r="A10" s="2"/>
@@ -1046,25 +1060,25 @@
       <c r="C10" s="7">
         <v>20</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="16">
         <v>30</v>
       </c>
       <c r="E10" s="8">
         <v>15</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="10">
         <v>30</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="12">
         <v>20</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="10">
         <v>30</v>
       </c>
       <c r="I10" s="8">
         <v>5</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="9">
         <v>10</v>
       </c>
     </row>
@@ -1078,25 +1092,25 @@
       <c r="C11" s="3">
         <v>11</v>
       </c>
-      <c r="D11" s="26">
+      <c r="D11" s="17">
         <v>15</v>
       </c>
       <c r="E11" s="6">
         <v>12</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="14">
         <v>15</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="13">
         <v>13</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="14">
         <v>15</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="41">
         <v>15</v>
       </c>
-      <c r="J11" s="13"/>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:10" ht="31">
       <c r="A12" s="2"/>
@@ -1106,69 +1120,69 @@
       <c r="C12" s="7">
         <v>11</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="16">
         <v>15</v>
       </c>
       <c r="E12" s="8">
         <v>12</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="10">
         <v>15</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="12">
         <v>13</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="10">
         <v>15</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="39">
         <v>15</v>
       </c>
-      <c r="J12" s="11"/>
+      <c r="J12" s="40"/>
     </row>
     <row r="13" spans="1:10" ht="31">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="10">
-        <v>3</v>
-      </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="10">
-        <v>3</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="18">
-        <v>3</v>
-      </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="10">
+      <c r="C13" s="39">
+        <v>3</v>
+      </c>
+      <c r="D13" s="47"/>
+      <c r="E13" s="39">
+        <v>3</v>
+      </c>
+      <c r="F13" s="44"/>
+      <c r="G13" s="43">
+        <v>3</v>
+      </c>
+      <c r="H13" s="44"/>
+      <c r="I13" s="39">
         <v>5</v>
       </c>
-      <c r="J13" s="11"/>
+      <c r="J13" s="40"/>
     </row>
     <row r="14" spans="1:10" ht="31">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="10">
-        <v>3</v>
-      </c>
-      <c r="D14" s="23"/>
-      <c r="E14" s="10">
-        <v>3</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="18">
-        <v>3</v>
-      </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="10">
+      <c r="C14" s="39">
+        <v>3</v>
+      </c>
+      <c r="D14" s="47"/>
+      <c r="E14" s="39">
+        <v>3</v>
+      </c>
+      <c r="F14" s="44"/>
+      <c r="G14" s="43">
+        <v>3</v>
+      </c>
+      <c r="H14" s="44"/>
+      <c r="I14" s="39">
         <v>5</v>
       </c>
-      <c r="J14" s="11"/>
+      <c r="J14" s="40"/>
     </row>
     <row r="15" spans="1:10" ht="31">
       <c r="A15" s="2"/>
@@ -1178,70 +1192,70 @@
       <c r="C15" s="7">
         <v>7</v>
       </c>
-      <c r="D15" s="25">
-        <v>3</v>
-      </c>
-      <c r="E15" s="10">
-        <v>0</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="18">
-        <v>0</v>
-      </c>
-      <c r="H15" s="14"/>
-      <c r="I15" s="10">
+      <c r="D15" s="16">
+        <v>3</v>
+      </c>
+      <c r="E15" s="39">
+        <v>0</v>
+      </c>
+      <c r="F15" s="44"/>
+      <c r="G15" s="43">
+        <v>0</v>
+      </c>
+      <c r="H15" s="44"/>
+      <c r="I15" s="39">
         <v>5</v>
       </c>
-      <c r="J15" s="11"/>
+      <c r="J15" s="40"/>
     </row>
     <row r="16" spans="1:10" ht="31">
       <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="11">
         <v>7</v>
       </c>
-      <c r="D16" s="27">
-        <v>3</v>
-      </c>
-      <c r="E16" s="10">
-        <v>0</v>
-      </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="18">
-        <v>0</v>
-      </c>
-      <c r="H16" s="14"/>
-      <c r="I16" s="10">
-        <v>0</v>
-      </c>
-      <c r="J16" s="11"/>
+      <c r="D16" s="18">
+        <v>3</v>
+      </c>
+      <c r="E16" s="39">
+        <v>0</v>
+      </c>
+      <c r="F16" s="44"/>
+      <c r="G16" s="43">
+        <v>0</v>
+      </c>
+      <c r="H16" s="44"/>
+      <c r="I16" s="39">
+        <v>0</v>
+      </c>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10" ht="31">
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="10">
-        <v>0</v>
-      </c>
-      <c r="D17" s="23"/>
+      <c r="C17" s="39">
+        <v>0</v>
+      </c>
+      <c r="D17" s="47"/>
       <c r="E17" s="8">
         <v>9</v>
       </c>
-      <c r="F17" s="15">
-        <v>3</v>
-      </c>
-      <c r="G17" s="19">
+      <c r="F17" s="10">
+        <v>3</v>
+      </c>
+      <c r="G17" s="12">
         <v>7</v>
       </c>
-      <c r="H17" s="15">
-        <v>3</v>
-      </c>
-      <c r="I17" s="10">
-        <v>0</v>
-      </c>
-      <c r="J17" s="11"/>
+      <c r="H17" s="10">
+        <v>3</v>
+      </c>
+      <c r="I17" s="39">
+        <v>0</v>
+      </c>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10" ht="31">
       <c r="A18" s="3" t="s">
@@ -1250,44 +1264,44 @@
       <c r="B18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="41">
         <v>0.1</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="9">
+      <c r="D18" s="48"/>
+      <c r="E18" s="41">
         <v>0.1</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="22">
+      <c r="F18" s="46"/>
+      <c r="G18" s="45">
         <v>0.1</v>
       </c>
-      <c r="H18" s="17"/>
-      <c r="I18" s="9">
+      <c r="H18" s="46"/>
+      <c r="I18" s="41">
         <v>1</v>
       </c>
-      <c r="J18" s="13"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" ht="31">
       <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="39">
         <v>0.1</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="10">
+      <c r="D19" s="47"/>
+      <c r="E19" s="39">
         <v>0.1</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="18">
+      <c r="F19" s="44"/>
+      <c r="G19" s="43">
         <v>0.1</v>
       </c>
-      <c r="H19" s="14"/>
-      <c r="I19" s="10">
+      <c r="H19" s="44"/>
+      <c r="I19" s="39">
         <v>0.2</v>
       </c>
-      <c r="J19" s="11"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" spans="1:10" ht="31">
       <c r="A20" s="1"/>
@@ -1335,37 +1349,7 @@
       <c r="C28" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="C9:D9"/>
+  <mergeCells count="44">
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
@@ -1381,6 +1365,35 @@
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I9:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1390,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08363EBC-35EB-8D4A-94A4-8966FDA7430E}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="47" zoomScaleNormal="47" workbookViewId="0">
-      <selection activeCell="J19" sqref="A1:J19"/>
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1415,46 +1428,46 @@
       <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="23"/>
-      <c r="E1" s="29" t="s">
+      <c r="D1" s="47"/>
+      <c r="E1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="29" t="s">
+      <c r="F1" s="47"/>
+      <c r="G1" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="29" t="s">
+      <c r="H1" s="47"/>
+      <c r="I1" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="23"/>
+      <c r="J1" s="47"/>
     </row>
     <row r="2" spans="1:10" ht="31">
       <c r="C2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1465,32 +1478,32 @@
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="38">
+      <c r="C3" s="27">
         <f>25/104.2</f>
         <v>0.23992322456813819</v>
       </c>
-      <c r="D3" s="32">
-        <v>0</v>
-      </c>
-      <c r="E3" s="38">
+      <c r="D3" s="21">
+        <v>0</v>
+      </c>
+      <c r="E3" s="27">
         <f>25/111.2</f>
         <v>0.22482014388489208</v>
       </c>
-      <c r="F3" s="32">
-        <v>0</v>
-      </c>
-      <c r="G3" s="31">
+      <c r="F3" s="21">
+        <v>0</v>
+      </c>
+      <c r="G3" s="20">
         <f>25/112.2</f>
         <v>0.22281639928698752</v>
       </c>
-      <c r="H3" s="32">
-        <v>0</v>
-      </c>
-      <c r="I3" s="31">
+      <c r="H3" s="21">
+        <v>0</v>
+      </c>
+      <c r="I3" s="20">
         <f>25/112.2</f>
         <v>0.22281639928698752</v>
       </c>
-      <c r="J3" s="32">
+      <c r="J3" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1499,35 +1512,35 @@
       <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="27">
         <f>10/104.2</f>
         <v>9.5969289827255277E-2</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="21">
         <f>30/104.2</f>
         <v>0.28790786948176583</v>
       </c>
-      <c r="E4" s="38">
+      <c r="E4" s="27">
         <f>15/111.2</f>
         <v>0.13489208633093525</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="21">
         <f>30/111.2</f>
         <v>0.26978417266187049</v>
       </c>
-      <c r="G4" s="31">
+      <c r="G4" s="20">
         <f>15/112.2</f>
         <v>0.13368983957219252</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="21">
         <f>30/112.2</f>
         <v>0.26737967914438504</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="20">
         <f>15/112.2</f>
         <v>0.13368983957219252</v>
       </c>
-      <c r="J4" s="32">
+      <c r="J4" s="21">
         <f>30/112.2</f>
         <v>0.26737967914438504</v>
       </c>
@@ -1537,35 +1550,35 @@
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="27">
         <f>3/104.2</f>
         <v>2.8790786948176581E-2</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="21">
         <f>3/104.2</f>
         <v>2.8790786948176581E-2</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="27">
         <f>3/111.2</f>
         <v>2.6978417266187049E-2</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="21">
         <f>3/111.2</f>
         <v>2.6978417266187049E-2</v>
       </c>
-      <c r="G5" s="31">
+      <c r="G5" s="20">
         <f>3/112.2</f>
         <v>2.6737967914438502E-2</v>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="21">
         <f>3/112.2</f>
         <v>2.6737967914438502E-2</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="20">
         <f>3/112.2</f>
         <v>2.6737967914438502E-2</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="21">
         <f>3/112.2</f>
         <v>2.6737967914438502E-2</v>
       </c>
@@ -1574,31 +1587,31 @@
       <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="39">
-        <v>0</v>
-      </c>
-      <c r="D6" s="34">
-        <v>0</v>
-      </c>
-      <c r="E6" s="38">
-        <v>0</v>
-      </c>
-      <c r="F6" s="32">
-        <v>0</v>
-      </c>
-      <c r="G6" s="31">
+      <c r="C6" s="28">
+        <v>0</v>
+      </c>
+      <c r="D6" s="23">
+        <v>0</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0</v>
+      </c>
+      <c r="F6" s="21">
+        <v>0</v>
+      </c>
+      <c r="G6" s="20">
         <f>4/112.2</f>
         <v>3.5650623885918005E-2</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="21">
         <f>1/112.2</f>
         <v>8.9126559714795012E-3</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I6" s="20">
         <f>1/112.2</f>
         <v>8.9126559714795012E-3</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="21">
         <f>1/112.2</f>
         <v>8.9126559714795012E-3</v>
       </c>
@@ -1607,32 +1620,32 @@
       <c r="B7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="39">
-        <v>0</v>
-      </c>
-      <c r="D7" s="34">
-        <v>0</v>
-      </c>
-      <c r="E7" s="38">
-        <v>0</v>
-      </c>
-      <c r="F7" s="32">
-        <v>0</v>
-      </c>
-      <c r="G7" s="31">
+      <c r="C7" s="28">
+        <v>0</v>
+      </c>
+      <c r="D7" s="23">
+        <v>0</v>
+      </c>
+      <c r="E7" s="27">
+        <v>0</v>
+      </c>
+      <c r="F7" s="21">
+        <v>0</v>
+      </c>
+      <c r="G7" s="20">
         <f>5/112.2</f>
         <v>4.4563279857397504E-2</v>
       </c>
-      <c r="H7" s="32">
-        <f>3/112.2</f>
-        <v>2.6737967914438502E-2</v>
-      </c>
-      <c r="I7" s="31">
-        <f>3/112.2</f>
-        <v>2.6737967914438502E-2</v>
-      </c>
-      <c r="J7" s="32">
-        <f>3/112.2</f>
+      <c r="H7" s="21">
+        <f t="shared" ref="H7:J9" si="0">3/112.2</f>
+        <v>2.6737967914438502E-2</v>
+      </c>
+      <c r="I7" s="20">
+        <f t="shared" si="0"/>
+        <v>2.6737967914438502E-2</v>
+      </c>
+      <c r="J7" s="21">
+        <f t="shared" si="0"/>
         <v>2.6737967914438502E-2</v>
       </c>
     </row>
@@ -1641,36 +1654,36 @@
       <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="28">
         <f>10/104.2</f>
         <v>9.5969289827255277E-2</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="23">
         <f>10/104.2</f>
         <v>9.5969289827255277E-2</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="27">
         <f>3/111.2</f>
         <v>2.6978417266187049E-2</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="21">
         <f>3/111.2</f>
         <v>2.6978417266187049E-2</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="20">
         <f>3/112.2</f>
         <v>2.6737967914438502E-2</v>
       </c>
-      <c r="H8" s="32">
-        <f>3/112.2</f>
-        <v>2.6737967914438502E-2</v>
-      </c>
-      <c r="I8" s="31">
-        <f>3/112.2</f>
-        <v>2.6737967914438502E-2</v>
-      </c>
-      <c r="J8" s="32">
-        <f>3/112.2</f>
+      <c r="H8" s="21">
+        <f t="shared" si="0"/>
+        <v>2.6737967914438502E-2</v>
+      </c>
+      <c r="I8" s="20">
+        <f t="shared" si="0"/>
+        <v>2.6737967914438502E-2</v>
+      </c>
+      <c r="J8" s="21">
+        <f t="shared" si="0"/>
         <v>2.6737967914438502E-2</v>
       </c>
     </row>
@@ -1679,36 +1692,36 @@
       <c r="B9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="28">
         <f>5/104.2</f>
         <v>4.7984644913627639E-2</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="23">
         <f>5/104.2</f>
         <v>4.7984644913627639E-2</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="27">
         <f>3/111.2</f>
         <v>2.6978417266187049E-2</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="21">
         <f>3/111.2</f>
         <v>2.6978417266187049E-2</v>
       </c>
-      <c r="G9" s="31">
+      <c r="G9" s="20">
         <f>3/112.2</f>
         <v>2.6737967914438502E-2</v>
       </c>
-      <c r="H9" s="32">
-        <f>3/112.2</f>
-        <v>2.6737967914438502E-2</v>
-      </c>
-      <c r="I9" s="31">
-        <f>3/112.2</f>
-        <v>2.6737967914438502E-2</v>
-      </c>
-      <c r="J9" s="32">
-        <f>3/112.2</f>
+      <c r="H9" s="21">
+        <f t="shared" si="0"/>
+        <v>2.6737967914438502E-2</v>
+      </c>
+      <c r="I9" s="20">
+        <f t="shared" si="0"/>
+        <v>2.6737967914438502E-2</v>
+      </c>
+      <c r="J9" s="21">
+        <f t="shared" si="0"/>
         <v>2.6737967914438502E-2</v>
       </c>
     </row>
@@ -1717,35 +1730,35 @@
       <c r="B10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="33">
         <f>5/104.2</f>
         <v>4.7984644913627639E-2</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="34">
         <f>10/104.2</f>
         <v>9.5969289827255277E-2</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="27">
         <f>20/111.2</f>
         <v>0.17985611510791366</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="21">
         <f>30/111.2</f>
         <v>0.26978417266187049</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="35">
         <f>15/112.2</f>
         <v>0.13368983957219252</v>
       </c>
-      <c r="H10" s="45">
+      <c r="H10" s="34">
         <f>30/112.2</f>
         <v>0.26737967914438504</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="20">
         <f>20/112.2</f>
         <v>0.17825311942959002</v>
       </c>
-      <c r="J10" s="32">
+      <c r="J10" s="21">
         <f>30/112.2</f>
         <v>0.26737967914438504</v>
       </c>
@@ -1757,35 +1770,35 @@
       <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="28">
         <f>15/104.2</f>
         <v>0.14395393474088292</v>
       </c>
-      <c r="D11" s="47">
+      <c r="D11" s="36">
         <f>15/104.2</f>
         <v>0.14395393474088292</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="29">
         <f>11/111.2</f>
         <v>9.8920863309352514E-2</v>
       </c>
-      <c r="F11" s="36">
+      <c r="F11" s="25">
         <f>15/111.2</f>
         <v>0.13489208633093525</v>
       </c>
-      <c r="G11" s="31">
+      <c r="G11" s="20">
         <f>12/112.2</f>
         <v>0.10695187165775401</v>
       </c>
-      <c r="H11" s="32">
+      <c r="H11" s="21">
         <f>15/112.2</f>
         <v>0.13368983957219252</v>
       </c>
-      <c r="I11" s="35">
+      <c r="I11" s="24">
         <f>13/112.2</f>
         <v>0.11586452762923351</v>
       </c>
-      <c r="J11" s="36">
+      <c r="J11" s="25">
         <f>15/112.2</f>
         <v>0.13368983957219252</v>
       </c>
@@ -1795,35 +1808,35 @@
       <c r="B12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="39">
+      <c r="C12" s="28">
         <f>15/104.2</f>
         <v>0.14395393474088292</v>
       </c>
-      <c r="D12" s="34">
+      <c r="D12" s="23">
         <f>15/104.2</f>
         <v>0.14395393474088292</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="27">
         <f>11/111.2</f>
         <v>9.8920863309352514E-2</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="21">
         <f>15/111.2</f>
         <v>0.13489208633093525</v>
       </c>
-      <c r="G12" s="31">
+      <c r="G12" s="20">
         <f>12/112.2</f>
         <v>0.10695187165775401</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="21">
         <f>15/112.2</f>
         <v>0.13368983957219252</v>
       </c>
-      <c r="I12" s="31">
+      <c r="I12" s="20">
         <f>13/112.2</f>
         <v>0.11586452762923351</v>
       </c>
-      <c r="J12" s="32">
+      <c r="J12" s="21">
         <f>15/112.2</f>
         <v>0.13368983957219252</v>
       </c>
@@ -1833,36 +1846,36 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="39">
-        <f>5/104.2</f>
+      <c r="C13" s="28">
+        <f t="shared" ref="C13:D15" si="1">5/104.2</f>
         <v>4.7984644913627639E-2</v>
       </c>
-      <c r="D13" s="34">
-        <f>5/104.2</f>
+      <c r="D13" s="23">
+        <f t="shared" si="1"/>
         <v>4.7984644913627639E-2</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="27">
         <f>3/111.2</f>
         <v>2.6978417266187049E-2</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="21">
         <f>3/111.2</f>
         <v>2.6978417266187049E-2</v>
       </c>
-      <c r="G13" s="31">
-        <f>3/112.2</f>
-        <v>2.6737967914438502E-2</v>
-      </c>
-      <c r="H13" s="32">
-        <f>3/112.2</f>
-        <v>2.6737967914438502E-2</v>
-      </c>
-      <c r="I13" s="31">
-        <f>3/112.2</f>
-        <v>2.6737967914438502E-2</v>
-      </c>
-      <c r="J13" s="48">
-        <f>3/112.2</f>
+      <c r="G13" s="20">
+        <f t="shared" ref="G13:J14" si="2">3/112.2</f>
+        <v>2.6737967914438502E-2</v>
+      </c>
+      <c r="H13" s="21">
+        <f t="shared" si="2"/>
+        <v>2.6737967914438502E-2</v>
+      </c>
+      <c r="I13" s="20">
+        <f t="shared" si="2"/>
+        <v>2.6737967914438502E-2</v>
+      </c>
+      <c r="J13" s="37">
+        <f t="shared" si="2"/>
         <v>2.6737967914438502E-2</v>
       </c>
     </row>
@@ -1871,36 +1884,36 @@
       <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="39">
-        <f>5/104.2</f>
+      <c r="C14" s="28">
+        <f t="shared" si="1"/>
         <v>4.7984644913627639E-2</v>
       </c>
-      <c r="D14" s="34">
-        <f>5/104.2</f>
+      <c r="D14" s="23">
+        <f t="shared" si="1"/>
         <v>4.7984644913627639E-2</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="27">
         <f>3/111.2</f>
         <v>2.6978417266187049E-2</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="21">
         <f>3/111.2</f>
         <v>2.6978417266187049E-2</v>
       </c>
-      <c r="G14" s="31">
-        <f>3/112.2</f>
-        <v>2.6737967914438502E-2</v>
-      </c>
-      <c r="H14" s="32">
-        <f>3/112.2</f>
-        <v>2.6737967914438502E-2</v>
-      </c>
-      <c r="I14" s="31">
-        <f>3/112.2</f>
-        <v>2.6737967914438502E-2</v>
-      </c>
-      <c r="J14" s="32">
-        <f>3/112.2</f>
+      <c r="G14" s="20">
+        <f t="shared" si="2"/>
+        <v>2.6737967914438502E-2</v>
+      </c>
+      <c r="H14" s="21">
+        <f t="shared" si="2"/>
+        <v>2.6737967914438502E-2</v>
+      </c>
+      <c r="I14" s="20">
+        <f t="shared" si="2"/>
+        <v>2.6737967914438502E-2</v>
+      </c>
+      <c r="J14" s="21">
+        <f t="shared" si="2"/>
         <v>2.6737967914438502E-2</v>
       </c>
     </row>
@@ -1909,32 +1922,32 @@
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="39">
-        <f>5/104.2</f>
+      <c r="C15" s="28">
+        <f t="shared" si="1"/>
         <v>4.7984644913627639E-2</v>
       </c>
-      <c r="D15" s="34">
-        <f>5/104.2</f>
+      <c r="D15" s="23">
+        <f t="shared" si="1"/>
         <v>4.7984644913627639E-2</v>
       </c>
-      <c r="E15" s="38">
+      <c r="E15" s="27">
         <f>7/111.2</f>
         <v>6.2949640287769781E-2</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="21">
         <f>3/111.2</f>
         <v>2.6978417266187049E-2</v>
       </c>
-      <c r="G15" s="31">
-        <v>0</v>
-      </c>
-      <c r="H15" s="32">
-        <v>0</v>
-      </c>
-      <c r="I15" s="31">
-        <v>0</v>
-      </c>
-      <c r="J15" s="32">
+      <c r="G15" s="20">
+        <v>0</v>
+      </c>
+      <c r="H15" s="21">
+        <v>0</v>
+      </c>
+      <c r="I15" s="20">
+        <v>0</v>
+      </c>
+      <c r="J15" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1943,30 +1956,30 @@
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="39">
-        <v>0</v>
-      </c>
-      <c r="D16" s="34">
-        <v>0</v>
-      </c>
-      <c r="E16" s="41">
+      <c r="C16" s="28">
+        <v>0</v>
+      </c>
+      <c r="D16" s="23">
+        <v>0</v>
+      </c>
+      <c r="E16" s="30">
         <f>7/111.2</f>
         <v>6.2949640287769781E-2</v>
       </c>
-      <c r="F16" s="42">
+      <c r="F16" s="31">
         <f>3/111.2</f>
         <v>2.6978417266187049E-2</v>
       </c>
-      <c r="G16" s="31">
-        <v>0</v>
-      </c>
-      <c r="H16" s="32">
-        <v>0</v>
-      </c>
-      <c r="I16" s="31">
-        <v>0</v>
-      </c>
-      <c r="J16" s="32">
+      <c r="G16" s="20">
+        <v>0</v>
+      </c>
+      <c r="H16" s="21">
+        <v>0</v>
+      </c>
+      <c r="I16" s="20">
+        <v>0</v>
+      </c>
+      <c r="J16" s="21">
         <v>0</v>
       </c>
     </row>
@@ -1974,31 +1987,31 @@
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="49">
-        <v>0</v>
-      </c>
-      <c r="D17" s="33">
-        <v>0</v>
-      </c>
-      <c r="E17" s="38">
-        <v>0</v>
-      </c>
-      <c r="F17" s="32">
-        <v>0</v>
-      </c>
-      <c r="G17" s="31">
+      <c r="C17" s="38">
+        <v>0</v>
+      </c>
+      <c r="D17" s="22">
+        <v>0</v>
+      </c>
+      <c r="E17" s="27">
+        <v>0</v>
+      </c>
+      <c r="F17" s="21">
+        <v>0</v>
+      </c>
+      <c r="G17" s="20">
         <f>9/112.2</f>
         <v>8.0213903743315509E-2</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="21">
         <f>3/112.2</f>
         <v>2.6737967914438502E-2</v>
       </c>
-      <c r="I17" s="31">
+      <c r="I17" s="20">
         <f>7/112.2</f>
         <v>6.2388591800356503E-2</v>
       </c>
-      <c r="J17" s="32">
+      <c r="J17" s="21">
         <f>3/112.2</f>
         <v>2.6737967914438502E-2</v>
       </c>
@@ -2010,36 +2023,36 @@
       <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="39">
+      <c r="C18" s="28">
         <f>1/104.2</f>
         <v>9.5969289827255271E-3</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="23">
         <f>1/104.2</f>
         <v>9.5969289827255271E-3</v>
       </c>
-      <c r="E18" s="40">
+      <c r="E18" s="29">
         <f>0.1/111.2</f>
         <v>8.9928057553956839E-4</v>
       </c>
-      <c r="F18" s="36">
+      <c r="F18" s="25">
         <f>0.1/111.2</f>
         <v>8.9928057553956839E-4</v>
       </c>
-      <c r="G18" s="35">
-        <f>0.1/112.2</f>
+      <c r="G18" s="24">
+        <f t="shared" ref="G18:J19" si="3">0.1/112.2</f>
         <v>8.9126559714795015E-4</v>
       </c>
-      <c r="H18" s="35">
-        <f>0.1/112.2</f>
+      <c r="H18" s="24">
+        <f t="shared" si="3"/>
         <v>8.9126559714795015E-4</v>
       </c>
-      <c r="I18" s="35">
-        <f>0.1/112.2</f>
+      <c r="I18" s="24">
+        <f t="shared" si="3"/>
         <v>8.9126559714795015E-4</v>
       </c>
-      <c r="J18" s="35">
-        <f>0.1/112.2</f>
+      <c r="J18" s="24">
+        <f t="shared" si="3"/>
         <v>8.9126559714795015E-4</v>
       </c>
     </row>
@@ -2048,36 +2061,36 @@
       <c r="B19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="28">
         <f>0.2/104.2</f>
         <v>1.9193857965451057E-3</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D19" s="23">
         <f>0.2/104.2</f>
         <v>1.9193857965451057E-3</v>
       </c>
-      <c r="E19" s="38">
+      <c r="E19" s="27">
         <f>0.1/111.2</f>
         <v>8.9928057553956839E-4</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="21">
         <f>0.1/111.2</f>
         <v>8.9928057553956839E-4</v>
       </c>
-      <c r="G19" s="31">
-        <f>0.1/112.2</f>
+      <c r="G19" s="20">
+        <f t="shared" si="3"/>
         <v>8.9126559714795015E-4</v>
       </c>
-      <c r="H19" s="31">
-        <f>0.1/112.2</f>
+      <c r="H19" s="20">
+        <f t="shared" si="3"/>
         <v>8.9126559714795015E-4</v>
       </c>
-      <c r="I19" s="31">
-        <f>0.1/112.2</f>
+      <c r="I19" s="20">
+        <f t="shared" si="3"/>
         <v>8.9126559714795015E-4</v>
       </c>
-      <c r="J19" s="31">
-        <f>0.1/112.2</f>
+      <c r="J19" s="20">
+        <f t="shared" si="3"/>
         <v>8.9126559714795015E-4</v>
       </c>
     </row>
@@ -2091,10 +2104,10 @@
     </row>
     <row r="21" spans="1:10" ht="31">
       <c r="C21" s="7"/>
-      <c r="E21" s="37"/>
-      <c r="G21" s="37"/>
+      <c r="E21" s="26"/>
+      <c r="G21" s="26"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="43"/>
+      <c r="I21" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>